<commit_message>
Fix backend script to start both frontend and backend together
</commit_message>
<xml_diff>
--- a/backend/Tunisian_Companies_Emails_Combined.xlsx
+++ b/backend/Tunisian_Companies_Emails_Combined.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="318">
-  <si>
-    <t>NOM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="322">
+  <si>
+    <t>nom</t>
   </si>
   <si>
     <t>EMAIL</t>
@@ -966,6 +966,18 @@
   </si>
   <si>
     <t>support@micro1.ai</t>
+  </si>
+  <si>
+    <t>ats-digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recrutement@ats-digital.com</t>
+  </si>
+  <si>
+    <t>tradrly</t>
+  </si>
+  <si>
+    <t>tradrlyjob@gmail.com</t>
   </si>
   <si>
     <t>SHOP MY INFLUENCE</t>
@@ -1318,7 +1330,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B168"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -2648,6 +2660,30 @@
         <v>317</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
+      <c r="A166" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
+      <c r="A167" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
+      <c r="A168" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>